<commit_message>
data generation for map viz
</commit_message>
<xml_diff>
--- a/raw/data/business_data_20210510.xlsx
+++ b/raw/data/business_data_20210510.xlsx
@@ -854,10 +854,10 @@
     <t xml:space="preserve">m_coodinates</t>
   </si>
   <si>
-    <t xml:space="preserve">_m_coodinates_latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_m_coodinates_longitude</t>
+    <t xml:space="preserve">m_coodinates_latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m_coodinates_longitude</t>
   </si>
   <si>
     <t xml:space="preserve">_m_coodinates_altitude</t>
@@ -5896,8 +5896,8 @@
   </sheetPr>
   <dimension ref="A1:KX109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="GI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="GS1" activeCellId="1" sqref="X1:Z1 GQ1:GS1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="JJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="JR1" activeCellId="0" sqref="JR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -70201,7 +70201,7 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="2" sqref="X1:Z1 GQ1:GS1 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>